<commit_message>
Updated README to match ratings ingest
</commit_message>
<xml_diff>
--- a/bracket_template.xlsx
+++ b/bracket_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Bracket" sheetId="1" state="visible" r:id="rId2"/>
@@ -69,7 +69,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -122,6 +122,20 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Serif"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Serif"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="7"/>
       <color rgb="FFFFFFFF"/>
       <name val="DejaVu Serif"/>
@@ -143,7 +157,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -332,14 +346,28 @@
       <left style="hair"/>
       <right/>
       <top/>
-      <bottom style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -368,7 +396,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="87">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -505,11 +533,51 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -517,23 +585,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -541,7 +605,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -597,15 +661,31 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -623,6 +703,14 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -633,12 +721,28 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -658,30 +762,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="1:73"/>
+  <dimension ref="A1:AMJ74"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F71" activeCellId="0" sqref="F71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q36" activeCellId="0" sqref="Q36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="0.748987854251012"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="2.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="1" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="0.748987854251012"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="0.748987854251012"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="0.748987854251012"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="3" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="3" width="0.748987854251012"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="3" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="3" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="2.78542510121457"/>
-    <col collapsed="false" hidden="false" max="257" min="20" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="4" width="8.78542510121457"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="0.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="2.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="10.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="0.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="0.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="10.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="0.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="10.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="0.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="3" width="10.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="2.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="257" min="20" style="1" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="258" style="4" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2951,7 +3055,7 @@
       <c r="B12" s="9"/>
       <c r="C12" s="26"/>
       <c r="D12" s="36"/>
-      <c r="E12" s="34"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
@@ -2962,8 +3066,8 @@
       <c r="M12" s="22"/>
       <c r="N12" s="22"/>
       <c r="O12" s="22"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="37"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="39"/>
       <c r="R12" s="28"/>
       <c r="S12" s="12"/>
     </row>
@@ -2972,8 +3076,8 @@
         <v>9</v>
       </c>
       <c r="C13" s="29"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="34"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="37"/>
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
@@ -2984,8 +3088,8 @@
       <c r="M13" s="25"/>
       <c r="N13" s="25"/>
       <c r="O13" s="25"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="25"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="40"/>
       <c r="R13" s="32"/>
       <c r="S13" s="12" t="n">
         <v>9</v>
@@ -2994,8 +3098,8 @@
     <row r="14" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="9"/>
       <c r="C14" s="33"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="34"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="37"/>
       <c r="F14" s="27"/>
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
@@ -3006,8 +3110,8 @@
       <c r="M14" s="25"/>
       <c r="N14" s="25"/>
       <c r="O14" s="27"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="25"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="40"/>
       <c r="R14" s="33"/>
       <c r="S14" s="12"/>
     </row>
@@ -3016,9 +3120,9 @@
         <v>5</v>
       </c>
       <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
+      <c r="D15" s="40"/>
       <c r="E15" s="25"/>
-      <c r="F15" s="38"/>
+      <c r="F15" s="41"/>
       <c r="G15" s="25"/>
       <c r="H15" s="25"/>
       <c r="I15" s="25"/>
@@ -3028,9 +3132,9 @@
       <c r="M15" s="25"/>
       <c r="N15" s="25"/>
       <c r="O15" s="31"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="39"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="42"/>
       <c r="S15" s="12" t="n">
         <v>5</v>
       </c>
@@ -3038,9 +3142,9 @@
     <row r="16" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="9"/>
       <c r="C16" s="26"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
@@ -3049,9 +3153,9 @@
       <c r="L16" s="25"/>
       <c r="M16" s="25"/>
       <c r="N16" s="25"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="27"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="43"/>
       <c r="R16" s="28"/>
       <c r="S16" s="12"/>
     </row>
@@ -3060,9 +3164,9 @@
         <v>12</v>
       </c>
       <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
       <c r="I17" s="25"/>
@@ -3071,9 +3175,9 @@
       <c r="L17" s="25"/>
       <c r="M17" s="25"/>
       <c r="N17" s="25"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="31"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="45"/>
       <c r="R17" s="32"/>
       <c r="S17" s="12" t="n">
         <v>12</v>
@@ -3083,18 +3187,18 @@
       <c r="B18" s="9"/>
       <c r="C18" s="33"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="34"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="37"/>
       <c r="G18" s="25"/>
       <c r="H18" s="25"/>
       <c r="I18" s="25"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
       <c r="L18" s="25"/>
       <c r="M18" s="25"/>
       <c r="N18" s="25"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="37"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="48"/>
       <c r="Q18" s="35"/>
       <c r="R18" s="33"/>
       <c r="S18" s="12"/>
@@ -3106,16 +3210,16 @@
       <c r="C19" s="24"/>
       <c r="D19" s="34"/>
       <c r="E19" s="25"/>
-      <c r="F19" s="34"/>
+      <c r="F19" s="37"/>
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
       <c r="I19" s="25"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
       <c r="L19" s="25"/>
       <c r="M19" s="25"/>
       <c r="N19" s="25"/>
-      <c r="O19" s="35"/>
+      <c r="O19" s="38"/>
       <c r="P19" s="25"/>
       <c r="Q19" s="35"/>
       <c r="R19" s="24"/>
@@ -3128,18 +3232,18 @@
       <c r="C20" s="26"/>
       <c r="D20" s="36"/>
       <c r="E20" s="25"/>
-      <c r="F20" s="34"/>
+      <c r="F20" s="37"/>
       <c r="G20" s="25"/>
       <c r="H20" s="25"/>
       <c r="I20" s="25"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
       <c r="L20" s="25"/>
       <c r="M20" s="25"/>
       <c r="N20" s="25"/>
-      <c r="O20" s="35"/>
+      <c r="O20" s="38"/>
       <c r="P20" s="25"/>
-      <c r="Q20" s="37"/>
+      <c r="Q20" s="39"/>
       <c r="R20" s="28"/>
       <c r="S20" s="12"/>
     </row>
@@ -3148,20 +3252,20 @@
         <v>13</v>
       </c>
       <c r="C21" s="29"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
       <c r="G21" s="11"/>
       <c r="H21" s="25"/>
       <c r="I21" s="25"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="40"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="41"/>
-      <c r="P21" s="41"/>
-      <c r="Q21" s="25"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="50"/>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="40"/>
       <c r="R21" s="32"/>
       <c r="S21" s="12" t="n">
         <v>13</v>
@@ -3170,20 +3274,20 @@
     <row r="22" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="9"/>
       <c r="C22" s="33"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
       <c r="I22" s="25"/>
       <c r="J22" s="25"/>
       <c r="K22" s="25"/>
       <c r="L22" s="25"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="41"/>
-      <c r="Q22" s="25"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="50"/>
+      <c r="P22" s="50"/>
+      <c r="Q22" s="40"/>
       <c r="R22" s="33"/>
       <c r="S22" s="12"/>
     </row>
@@ -3192,10 +3296,10 @@
         <v>6</v>
       </c>
       <c r="C23" s="24"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="42"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="51"/>
       <c r="H23" s="30"/>
       <c r="I23" s="25"/>
       <c r="J23" s="25"/>
@@ -3203,9 +3307,9 @@
       <c r="L23" s="25"/>
       <c r="M23" s="31"/>
       <c r="N23" s="30"/>
-      <c r="O23" s="41"/>
-      <c r="P23" s="41"/>
-      <c r="Q23" s="25"/>
+      <c r="O23" s="50"/>
+      <c r="P23" s="50"/>
+      <c r="Q23" s="40"/>
       <c r="R23" s="24"/>
       <c r="S23" s="12" t="n">
         <v>6</v>
@@ -3214,20 +3318,20 @@
     <row r="24" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="9"/>
       <c r="C24" s="26"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
       <c r="G24" s="25"/>
-      <c r="H24" s="34"/>
+      <c r="H24" s="37"/>
       <c r="I24" s="25"/>
       <c r="J24" s="25"/>
       <c r="K24" s="25"/>
       <c r="L24" s="25"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="41"/>
-      <c r="Q24" s="27"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="37"/>
+      <c r="O24" s="50"/>
+      <c r="P24" s="50"/>
+      <c r="Q24" s="43"/>
       <c r="R24" s="28"/>
       <c r="S24" s="12"/>
     </row>
@@ -3235,21 +3339,21 @@
       <c r="B25" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="C25" s="39"/>
-      <c r="D25" s="43"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="52"/>
       <c r="E25" s="25"/>
-      <c r="F25" s="34"/>
+      <c r="F25" s="37"/>
       <c r="G25" s="25"/>
-      <c r="H25" s="34"/>
+      <c r="H25" s="37"/>
       <c r="I25" s="25"/>
       <c r="J25" s="25"/>
       <c r="K25" s="25"/>
       <c r="L25" s="25"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="34"/>
-      <c r="O25" s="35"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="38"/>
       <c r="P25" s="25"/>
-      <c r="Q25" s="31"/>
+      <c r="Q25" s="45"/>
       <c r="R25" s="32"/>
       <c r="S25" s="12" t="n">
         <v>11</v>
@@ -3260,16 +3364,16 @@
       <c r="C26" s="33"/>
       <c r="D26" s="34"/>
       <c r="E26" s="27"/>
-      <c r="F26" s="34"/>
+      <c r="F26" s="37"/>
       <c r="G26" s="25"/>
-      <c r="H26" s="34"/>
+      <c r="H26" s="37"/>
       <c r="I26" s="25"/>
       <c r="J26" s="25"/>
       <c r="K26" s="25"/>
       <c r="L26" s="25"/>
-      <c r="M26" s="35"/>
-      <c r="N26" s="34"/>
-      <c r="O26" s="35"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="38"/>
       <c r="P26" s="27"/>
       <c r="Q26" s="35"/>
       <c r="R26" s="33"/>
@@ -3282,16 +3386,16 @@
       <c r="C27" s="24"/>
       <c r="D27" s="34"/>
       <c r="E27" s="30"/>
-      <c r="F27" s="44"/>
+      <c r="F27" s="53"/>
       <c r="G27" s="25"/>
-      <c r="H27" s="34"/>
+      <c r="H27" s="37"/>
       <c r="I27" s="25"/>
       <c r="J27" s="25"/>
       <c r="K27" s="25"/>
       <c r="L27" s="25"/>
-      <c r="M27" s="35"/>
-      <c r="N27" s="34"/>
-      <c r="O27" s="35"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="37"/>
+      <c r="O27" s="38"/>
       <c r="P27" s="31"/>
       <c r="Q27" s="35"/>
       <c r="R27" s="24"/>
@@ -3303,19 +3407,19 @@
       <c r="B28" s="9"/>
       <c r="C28" s="26"/>
       <c r="D28" s="36"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="44"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="53"/>
       <c r="G28" s="25"/>
-      <c r="H28" s="34"/>
+      <c r="H28" s="37"/>
       <c r="I28" s="25"/>
       <c r="J28" s="25"/>
       <c r="K28" s="25"/>
       <c r="L28" s="25"/>
-      <c r="M28" s="35"/>
-      <c r="N28" s="34"/>
-      <c r="O28" s="35"/>
-      <c r="P28" s="35"/>
-      <c r="Q28" s="37"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="37"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="38"/>
+      <c r="Q28" s="39"/>
       <c r="R28" s="28"/>
       <c r="S28" s="12"/>
     </row>
@@ -3324,20 +3428,20 @@
         <v>14</v>
       </c>
       <c r="C29" s="29"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="44"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="53"/>
       <c r="G29" s="25"/>
-      <c r="H29" s="34"/>
+      <c r="H29" s="37"/>
       <c r="I29" s="27"/>
       <c r="J29" s="27"/>
       <c r="K29" s="25"/>
       <c r="L29" s="25"/>
-      <c r="M29" s="35"/>
-      <c r="N29" s="34"/>
-      <c r="O29" s="35"/>
-      <c r="P29" s="35"/>
-      <c r="Q29" s="25"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="37"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="38"/>
+      <c r="Q29" s="40"/>
       <c r="R29" s="32"/>
       <c r="S29" s="12" t="n">
         <v>14</v>
@@ -3346,20 +3450,20 @@
     <row r="30" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="9"/>
       <c r="C30" s="33"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="45"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="54"/>
       <c r="G30" s="25"/>
       <c r="H30" s="25"/>
       <c r="I30" s="31"/>
-      <c r="J30" s="46"/>
+      <c r="J30" s="55"/>
       <c r="K30" s="25"/>
       <c r="L30" s="25"/>
-      <c r="M30" s="35"/>
-      <c r="N30" s="34"/>
-      <c r="O30" s="37"/>
-      <c r="P30" s="35"/>
-      <c r="Q30" s="25"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="37"/>
+      <c r="O30" s="48"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="40"/>
       <c r="R30" s="33"/>
       <c r="S30" s="12"/>
     </row>
@@ -3368,20 +3472,20 @@
         <v>7</v>
       </c>
       <c r="C31" s="24"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="34"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="37"/>
       <c r="F31" s="25"/>
       <c r="G31" s="25"/>
-      <c r="H31" s="34"/>
+      <c r="H31" s="37"/>
       <c r="I31" s="25"/>
       <c r="J31" s="25"/>
       <c r="K31" s="25"/>
       <c r="L31" s="25"/>
-      <c r="M31" s="35"/>
+      <c r="M31" s="38"/>
       <c r="N31" s="25"/>
       <c r="O31" s="25"/>
-      <c r="P31" s="35"/>
-      <c r="Q31" s="25"/>
+      <c r="P31" s="38"/>
+      <c r="Q31" s="40"/>
       <c r="R31" s="24"/>
       <c r="S31" s="12" t="n">
         <v>7</v>
@@ -3390,20 +3494,20 @@
     <row r="32" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="9"/>
       <c r="C32" s="26"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="34"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="37"/>
       <c r="F32" s="25"/>
       <c r="G32" s="25"/>
-      <c r="H32" s="34"/>
+      <c r="H32" s="37"/>
       <c r="I32" s="25"/>
       <c r="J32" s="25"/>
       <c r="K32" s="25"/>
       <c r="L32" s="25"/>
-      <c r="M32" s="35"/>
+      <c r="M32" s="38"/>
       <c r="N32" s="25"/>
       <c r="O32" s="25"/>
-      <c r="P32" s="35"/>
-      <c r="Q32" s="27"/>
+      <c r="P32" s="38"/>
+      <c r="Q32" s="43"/>
       <c r="R32" s="28"/>
       <c r="S32" s="12"/>
     </row>
@@ -3411,21 +3515,21 @@
       <c r="B33" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="C33" s="47"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="34"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="37"/>
       <c r="F33" s="25"/>
       <c r="G33" s="25"/>
-      <c r="H33" s="34"/>
+      <c r="H33" s="37"/>
       <c r="I33" s="25"/>
       <c r="J33" s="25"/>
       <c r="K33" s="25"/>
       <c r="L33" s="25"/>
-      <c r="M33" s="35"/>
+      <c r="M33" s="38"/>
       <c r="N33" s="25"/>
       <c r="O33" s="25"/>
-      <c r="P33" s="35"/>
-      <c r="Q33" s="31"/>
+      <c r="P33" s="38"/>
+      <c r="Q33" s="45"/>
       <c r="R33" s="32"/>
       <c r="S33" s="12" t="n">
         <v>10</v>
@@ -3435,18 +3539,18 @@
       <c r="B34" s="9"/>
       <c r="C34" s="33"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="36"/>
+      <c r="E34" s="46"/>
       <c r="F34" s="25"/>
       <c r="G34" s="25"/>
-      <c r="H34" s="34"/>
+      <c r="H34" s="37"/>
       <c r="I34" s="25"/>
       <c r="J34" s="25"/>
       <c r="K34" s="25"/>
       <c r="L34" s="25"/>
-      <c r="M34" s="35"/>
+      <c r="M34" s="38"/>
       <c r="N34" s="25"/>
       <c r="O34" s="25"/>
-      <c r="P34" s="37"/>
+      <c r="P34" s="48"/>
       <c r="Q34" s="35"/>
       <c r="R34" s="33"/>
       <c r="S34" s="12"/>
@@ -3460,12 +3564,12 @@
       <c r="E35" s="25"/>
       <c r="F35" s="25"/>
       <c r="G35" s="25"/>
-      <c r="H35" s="34"/>
+      <c r="H35" s="37"/>
       <c r="I35" s="25"/>
       <c r="J35" s="25"/>
       <c r="K35" s="25"/>
       <c r="L35" s="25"/>
-      <c r="M35" s="35"/>
+      <c r="M35" s="38"/>
       <c r="N35" s="25"/>
       <c r="O35" s="25"/>
       <c r="P35" s="25"/>
@@ -3480,20 +3584,20 @@
       <c r="C36" s="26"/>
       <c r="D36" s="36"/>
       <c r="E36" s="25"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="48"/>
-      <c r="H36" s="48"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
       <c r="I36" s="25"/>
-      <c r="J36" s="40" t="s">
+      <c r="J36" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="K36" s="40"/>
+      <c r="K36" s="47"/>
       <c r="L36" s="25"/>
-      <c r="M36" s="49"/>
-      <c r="N36" s="49"/>
-      <c r="O36" s="49"/>
+      <c r="M36" s="58"/>
+      <c r="N36" s="58"/>
+      <c r="O36" s="58"/>
       <c r="P36" s="25"/>
-      <c r="Q36" s="37"/>
+      <c r="Q36" s="39"/>
       <c r="R36" s="28"/>
       <c r="S36" s="12"/>
     </row>
@@ -3502,20 +3606,20 @@
         <v>15</v>
       </c>
       <c r="C37" s="29"/>
-      <c r="D37" s="25"/>
+      <c r="D37" s="40"/>
       <c r="E37" s="25"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="48"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
       <c r="I37" s="25"/>
-      <c r="J37" s="40"/>
-      <c r="K37" s="40"/>
+      <c r="J37" s="47"/>
+      <c r="K37" s="47"/>
       <c r="L37" s="25"/>
-      <c r="M37" s="49"/>
-      <c r="N37" s="49"/>
-      <c r="O37" s="49"/>
+      <c r="M37" s="58"/>
+      <c r="N37" s="58"/>
+      <c r="O37" s="58"/>
       <c r="P37" s="25"/>
-      <c r="Q37" s="25"/>
+      <c r="Q37" s="40"/>
       <c r="R37" s="32"/>
       <c r="S37" s="12" t="n">
         <v>15</v>
@@ -3524,20 +3628,20 @@
     <row r="38" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="9"/>
       <c r="C38" s="33"/>
-      <c r="D38" s="25"/>
+      <c r="D38" s="40"/>
       <c r="E38" s="25"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="48"/>
-      <c r="H38" s="48"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
       <c r="I38" s="25"/>
-      <c r="J38" s="40"/>
-      <c r="K38" s="40"/>
+      <c r="J38" s="47"/>
+      <c r="K38" s="47"/>
       <c r="L38" s="25"/>
-      <c r="M38" s="49"/>
-      <c r="N38" s="49"/>
-      <c r="O38" s="49"/>
+      <c r="M38" s="58"/>
+      <c r="N38" s="58"/>
+      <c r="O38" s="58"/>
       <c r="P38" s="25"/>
-      <c r="Q38" s="25"/>
+      <c r="Q38" s="40"/>
       <c r="R38" s="33"/>
       <c r="S38" s="12"/>
     </row>
@@ -3546,20 +3650,20 @@
         <v>1</v>
       </c>
       <c r="C39" s="24"/>
-      <c r="D39" s="25"/>
+      <c r="D39" s="40"/>
       <c r="E39" s="25"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="48"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="57"/>
+      <c r="H39" s="57"/>
       <c r="I39" s="25"/>
-      <c r="J39" s="50"/>
-      <c r="K39" s="50"/>
+      <c r="J39" s="59"/>
+      <c r="K39" s="59"/>
       <c r="L39" s="25"/>
-      <c r="M39" s="49"/>
-      <c r="N39" s="49"/>
-      <c r="O39" s="49"/>
+      <c r="M39" s="58"/>
+      <c r="N39" s="58"/>
+      <c r="O39" s="58"/>
       <c r="P39" s="25"/>
-      <c r="Q39" s="25"/>
+      <c r="Q39" s="40"/>
       <c r="R39" s="24"/>
       <c r="S39" s="12" t="n">
         <v>1</v>
@@ -3568,20 +3672,20 @@
     <row r="40" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="9"/>
       <c r="C40" s="26"/>
-      <c r="D40" s="27"/>
+      <c r="D40" s="43"/>
       <c r="E40" s="25"/>
-      <c r="F40" s="48"/>
-      <c r="G40" s="48"/>
-      <c r="H40" s="48"/>
+      <c r="F40" s="57"/>
+      <c r="G40" s="57"/>
+      <c r="H40" s="57"/>
       <c r="I40" s="25"/>
-      <c r="J40" s="50"/>
-      <c r="K40" s="50"/>
+      <c r="J40" s="59"/>
+      <c r="K40" s="59"/>
       <c r="L40" s="25"/>
-      <c r="M40" s="49"/>
-      <c r="N40" s="49"/>
-      <c r="O40" s="49"/>
+      <c r="M40" s="58"/>
+      <c r="N40" s="58"/>
+      <c r="O40" s="58"/>
       <c r="P40" s="25"/>
-      <c r="Q40" s="27"/>
+      <c r="Q40" s="43"/>
       <c r="R40" s="28"/>
       <c r="S40" s="12"/>
     </row>
@@ -3590,20 +3694,20 @@
         <v>16</v>
       </c>
       <c r="C41" s="29"/>
-      <c r="D41" s="30"/>
+      <c r="D41" s="44"/>
       <c r="E41" s="25"/>
       <c r="F41" s="25"/>
       <c r="G41" s="25"/>
-      <c r="H41" s="34"/>
+      <c r="H41" s="37"/>
       <c r="I41" s="25"/>
-      <c r="J41" s="50"/>
-      <c r="K41" s="50"/>
+      <c r="J41" s="59"/>
+      <c r="K41" s="59"/>
       <c r="L41" s="25"/>
-      <c r="M41" s="35"/>
+      <c r="M41" s="38"/>
       <c r="N41" s="25"/>
       <c r="O41" s="25"/>
       <c r="P41" s="25"/>
-      <c r="Q41" s="31"/>
+      <c r="Q41" s="45"/>
       <c r="R41" s="32"/>
       <c r="S41" s="12" t="n">
         <v>16</v>
@@ -3616,12 +3720,12 @@
       <c r="E42" s="27"/>
       <c r="F42" s="25"/>
       <c r="G42" s="25"/>
-      <c r="H42" s="34"/>
+      <c r="H42" s="37"/>
       <c r="I42" s="25"/>
       <c r="J42" s="11"/>
       <c r="K42" s="25"/>
       <c r="L42" s="25"/>
-      <c r="M42" s="35"/>
+      <c r="M42" s="38"/>
       <c r="N42" s="25"/>
       <c r="O42" s="25"/>
       <c r="P42" s="27"/>
@@ -3638,12 +3742,12 @@
       <c r="E43" s="30"/>
       <c r="F43" s="25"/>
       <c r="G43" s="25"/>
-      <c r="H43" s="34"/>
+      <c r="H43" s="37"/>
       <c r="I43" s="25"/>
       <c r="J43" s="25"/>
       <c r="K43" s="25"/>
       <c r="L43" s="25"/>
-      <c r="M43" s="35"/>
+      <c r="M43" s="38"/>
       <c r="N43" s="25"/>
       <c r="O43" s="25"/>
       <c r="P43" s="31"/>
@@ -3657,19 +3761,19 @@
       <c r="B44" s="9"/>
       <c r="C44" s="26"/>
       <c r="D44" s="36"/>
-      <c r="E44" s="34"/>
+      <c r="E44" s="37"/>
       <c r="F44" s="25"/>
       <c r="G44" s="25"/>
-      <c r="H44" s="34"/>
+      <c r="H44" s="37"/>
       <c r="I44" s="25"/>
       <c r="J44" s="25"/>
       <c r="K44" s="25"/>
       <c r="L44" s="25"/>
-      <c r="M44" s="35"/>
+      <c r="M44" s="38"/>
       <c r="N44" s="25"/>
       <c r="O44" s="25"/>
-      <c r="P44" s="35"/>
-      <c r="Q44" s="37"/>
+      <c r="P44" s="38"/>
+      <c r="Q44" s="39"/>
       <c r="R44" s="28"/>
       <c r="S44" s="12"/>
     </row>
@@ -3678,20 +3782,20 @@
         <v>9</v>
       </c>
       <c r="C45" s="29"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="34"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="37"/>
       <c r="F45" s="25"/>
       <c r="G45" s="25"/>
-      <c r="H45" s="34"/>
+      <c r="H45" s="37"/>
       <c r="I45" s="25"/>
       <c r="J45" s="25"/>
       <c r="K45" s="25"/>
       <c r="L45" s="25"/>
-      <c r="M45" s="35"/>
+      <c r="M45" s="38"/>
       <c r="N45" s="25"/>
       <c r="O45" s="25"/>
-      <c r="P45" s="35"/>
-      <c r="Q45" s="25"/>
+      <c r="P45" s="38"/>
+      <c r="Q45" s="40"/>
       <c r="R45" s="32"/>
       <c r="S45" s="12" t="n">
         <v>9</v>
@@ -3700,20 +3804,20 @@
     <row r="46" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="9"/>
       <c r="C46" s="33"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="34"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="37"/>
       <c r="F46" s="27"/>
       <c r="G46" s="25"/>
-      <c r="H46" s="34"/>
+      <c r="H46" s="37"/>
       <c r="I46" s="25"/>
       <c r="J46" s="25"/>
       <c r="K46" s="25"/>
       <c r="L46" s="25"/>
-      <c r="M46" s="35"/>
+      <c r="M46" s="38"/>
       <c r="N46" s="25"/>
       <c r="O46" s="27"/>
-      <c r="P46" s="35"/>
-      <c r="Q46" s="25"/>
+      <c r="P46" s="38"/>
+      <c r="Q46" s="40"/>
       <c r="R46" s="33"/>
       <c r="S46" s="12"/>
     </row>
@@ -3721,21 +3825,21 @@
       <c r="B47" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="C47" s="51"/>
-      <c r="D47" s="25"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="40"/>
       <c r="E47" s="25"/>
-      <c r="F47" s="38"/>
+      <c r="F47" s="41"/>
       <c r="G47" s="25"/>
-      <c r="H47" s="34"/>
+      <c r="H47" s="37"/>
       <c r="I47" s="25"/>
       <c r="J47" s="25"/>
-      <c r="K47" s="36"/>
-      <c r="L47" s="36"/>
-      <c r="M47" s="35"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="46"/>
+      <c r="M47" s="38"/>
       <c r="N47" s="25"/>
       <c r="O47" s="31"/>
-      <c r="P47" s="35"/>
-      <c r="Q47" s="25"/>
+      <c r="P47" s="38"/>
+      <c r="Q47" s="40"/>
       <c r="R47" s="24"/>
       <c r="S47" s="12" t="n">
         <v>5</v>
@@ -3744,20 +3848,20 @@
     <row r="48" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="9"/>
       <c r="C48" s="26"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
       <c r="G48" s="25"/>
-      <c r="H48" s="34"/>
+      <c r="H48" s="37"/>
       <c r="I48" s="25"/>
       <c r="J48" s="25"/>
       <c r="K48" s="10"/>
       <c r="L48" s="25"/>
-      <c r="M48" s="35"/>
-      <c r="N48" s="34"/>
-      <c r="O48" s="35"/>
-      <c r="P48" s="35"/>
-      <c r="Q48" s="27"/>
+      <c r="M48" s="38"/>
+      <c r="N48" s="37"/>
+      <c r="O48" s="38"/>
+      <c r="P48" s="38"/>
+      <c r="Q48" s="43"/>
       <c r="R48" s="28"/>
       <c r="S48" s="12"/>
     </row>
@@ -3765,21 +3869,21 @@
       <c r="B49" s="9" t="n">
         <v>12</v>
       </c>
-      <c r="C49" s="52"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
+      <c r="C49" s="61"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
       <c r="G49" s="25"/>
-      <c r="H49" s="34"/>
+      <c r="H49" s="37"/>
       <c r="I49" s="25"/>
       <c r="J49" s="25"/>
       <c r="K49" s="25"/>
       <c r="L49" s="25"/>
-      <c r="M49" s="35"/>
-      <c r="N49" s="34"/>
-      <c r="O49" s="35"/>
-      <c r="P49" s="35"/>
-      <c r="Q49" s="31"/>
+      <c r="M49" s="38"/>
+      <c r="N49" s="37"/>
+      <c r="O49" s="38"/>
+      <c r="P49" s="38"/>
+      <c r="Q49" s="45"/>
       <c r="R49" s="32"/>
       <c r="S49" s="12" t="n">
         <v>12</v>
@@ -3789,18 +3893,18 @@
       <c r="B50" s="9"/>
       <c r="C50" s="33"/>
       <c r="D50" s="34"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="34"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="37"/>
       <c r="G50" s="25"/>
-      <c r="H50" s="34"/>
+      <c r="H50" s="37"/>
       <c r="I50" s="25"/>
       <c r="J50" s="25"/>
       <c r="K50" s="25"/>
       <c r="L50" s="25"/>
-      <c r="M50" s="35"/>
-      <c r="N50" s="34"/>
-      <c r="O50" s="35"/>
-      <c r="P50" s="37"/>
+      <c r="M50" s="38"/>
+      <c r="N50" s="37"/>
+      <c r="O50" s="38"/>
+      <c r="P50" s="48"/>
       <c r="Q50" s="35"/>
       <c r="R50" s="33"/>
       <c r="S50" s="12"/>
@@ -3809,19 +3913,19 @@
       <c r="B51" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="C51" s="53"/>
+      <c r="C51" s="62"/>
       <c r="D51" s="34"/>
       <c r="E51" s="25"/>
-      <c r="F51" s="34"/>
+      <c r="F51" s="37"/>
       <c r="G51" s="25"/>
-      <c r="H51" s="34"/>
+      <c r="H51" s="37"/>
       <c r="I51" s="25"/>
       <c r="J51" s="25"/>
       <c r="K51" s="25"/>
       <c r="L51" s="25"/>
-      <c r="M51" s="35"/>
-      <c r="N51" s="34"/>
-      <c r="O51" s="35"/>
+      <c r="M51" s="38"/>
+      <c r="N51" s="37"/>
+      <c r="O51" s="38"/>
       <c r="P51" s="25"/>
       <c r="Q51" s="35"/>
       <c r="R51" s="24"/>
@@ -3834,18 +3938,18 @@
       <c r="C52" s="26"/>
       <c r="D52" s="36"/>
       <c r="E52" s="25"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="35"/>
-      <c r="H52" s="34"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="38"/>
+      <c r="H52" s="37"/>
       <c r="I52" s="25"/>
       <c r="J52" s="25"/>
       <c r="K52" s="25"/>
       <c r="L52" s="25"/>
-      <c r="M52" s="35"/>
-      <c r="N52" s="34"/>
-      <c r="O52" s="35"/>
+      <c r="M52" s="38"/>
+      <c r="N52" s="37"/>
+      <c r="O52" s="38"/>
       <c r="P52" s="25"/>
-      <c r="Q52" s="37"/>
+      <c r="Q52" s="39"/>
       <c r="R52" s="28"/>
       <c r="S52" s="12"/>
     </row>
@@ -3854,20 +3958,20 @@
         <v>13</v>
       </c>
       <c r="C53" s="29"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="54"/>
-      <c r="H53" s="34"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="49"/>
+      <c r="F53" s="49"/>
+      <c r="G53" s="63"/>
+      <c r="H53" s="37"/>
       <c r="I53" s="25"/>
-      <c r="J53" s="55"/>
-      <c r="K53" s="56"/>
+      <c r="J53" s="64"/>
+      <c r="K53" s="65"/>
       <c r="L53" s="25"/>
-      <c r="M53" s="35"/>
-      <c r="N53" s="34"/>
-      <c r="O53" s="14"/>
-      <c r="P53" s="14"/>
-      <c r="Q53" s="25"/>
+      <c r="M53" s="38"/>
+      <c r="N53" s="37"/>
+      <c r="O53" s="66"/>
+      <c r="P53" s="66"/>
+      <c r="Q53" s="40"/>
       <c r="R53" s="32"/>
       <c r="S53" s="12" t="n">
         <v>13</v>
@@ -3876,20 +3980,20 @@
     <row r="54" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="9"/>
       <c r="C54" s="33"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="45"/>
-      <c r="H54" s="45"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="54"/>
+      <c r="H54" s="54"/>
       <c r="I54" s="25"/>
-      <c r="J54" s="56"/>
-      <c r="K54" s="56"/>
+      <c r="J54" s="65"/>
+      <c r="K54" s="65"/>
       <c r="L54" s="25"/>
-      <c r="M54" s="45"/>
-      <c r="N54" s="45"/>
-      <c r="O54" s="14"/>
-      <c r="P54" s="14"/>
-      <c r="Q54" s="25"/>
+      <c r="M54" s="54"/>
+      <c r="N54" s="54"/>
+      <c r="O54" s="66"/>
+      <c r="P54" s="66"/>
+      <c r="Q54" s="40"/>
       <c r="R54" s="33"/>
       <c r="S54" s="12"/>
     </row>
@@ -3898,20 +4002,20 @@
         <v>6</v>
       </c>
       <c r="C55" s="24"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="49"/>
+      <c r="F55" s="49"/>
       <c r="G55" s="11"/>
       <c r="H55" s="25"/>
       <c r="I55" s="25"/>
-      <c r="J55" s="56"/>
-      <c r="K55" s="56"/>
+      <c r="J55" s="65"/>
+      <c r="K55" s="65"/>
       <c r="L55" s="25"/>
       <c r="M55" s="25"/>
       <c r="N55" s="25"/>
-      <c r="O55" s="14"/>
-      <c r="P55" s="14"/>
-      <c r="Q55" s="25"/>
+      <c r="O55" s="66"/>
+      <c r="P55" s="66"/>
+      <c r="Q55" s="40"/>
       <c r="R55" s="24"/>
       <c r="S55" s="12" t="n">
         <v>6</v>
@@ -3920,20 +4024,20 @@
     <row r="56" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="9"/>
       <c r="C56" s="26"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="49"/>
       <c r="G56" s="25"/>
       <c r="H56" s="25"/>
       <c r="I56" s="25"/>
-      <c r="J56" s="41"/>
-      <c r="K56" s="41"/>
+      <c r="J56" s="67"/>
+      <c r="K56" s="67"/>
       <c r="L56" s="25"/>
       <c r="M56" s="25"/>
       <c r="N56" s="25"/>
-      <c r="O56" s="14"/>
-      <c r="P56" s="14"/>
-      <c r="Q56" s="27"/>
+      <c r="O56" s="66"/>
+      <c r="P56" s="66"/>
+      <c r="Q56" s="43"/>
       <c r="R56" s="28"/>
       <c r="S56" s="12"/>
     </row>
@@ -3944,20 +4048,20 @@
       <c r="C57" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D57" s="30"/>
+      <c r="D57" s="44"/>
       <c r="E57" s="25"/>
-      <c r="F57" s="34"/>
+      <c r="F57" s="37"/>
       <c r="G57" s="25"/>
       <c r="H57" s="25"/>
       <c r="I57" s="25"/>
-      <c r="J57" s="41"/>
-      <c r="K57" s="41"/>
+      <c r="J57" s="67"/>
+      <c r="K57" s="67"/>
       <c r="L57" s="25"/>
       <c r="M57" s="25"/>
       <c r="N57" s="25"/>
-      <c r="O57" s="35"/>
+      <c r="O57" s="38"/>
       <c r="P57" s="25"/>
-      <c r="Q57" s="31"/>
+      <c r="Q57" s="45"/>
       <c r="R57" s="32" t="s">
         <v>10</v>
       </c>
@@ -3970,16 +4074,16 @@
       <c r="C58" s="33"/>
       <c r="D58" s="34"/>
       <c r="E58" s="27"/>
-      <c r="F58" s="34"/>
+      <c r="F58" s="37"/>
       <c r="G58" s="25"/>
       <c r="H58" s="25"/>
       <c r="I58" s="25"/>
-      <c r="J58" s="41"/>
-      <c r="K58" s="41"/>
+      <c r="J58" s="67"/>
+      <c r="K58" s="67"/>
       <c r="L58" s="25"/>
       <c r="M58" s="25"/>
       <c r="N58" s="25"/>
-      <c r="O58" s="35"/>
+      <c r="O58" s="38"/>
       <c r="P58" s="27"/>
       <c r="Q58" s="35"/>
       <c r="R58" s="33"/>
@@ -3992,16 +4096,16 @@
       <c r="C59" s="24"/>
       <c r="D59" s="34"/>
       <c r="E59" s="30"/>
-      <c r="F59" s="34"/>
+      <c r="F59" s="37"/>
       <c r="G59" s="25"/>
       <c r="H59" s="25"/>
       <c r="I59" s="25"/>
-      <c r="J59" s="41"/>
-      <c r="K59" s="41"/>
+      <c r="J59" s="67"/>
+      <c r="K59" s="67"/>
       <c r="L59" s="25"/>
       <c r="M59" s="25"/>
       <c r="N59" s="25"/>
-      <c r="O59" s="35"/>
+      <c r="O59" s="38"/>
       <c r="P59" s="31"/>
       <c r="Q59" s="35"/>
       <c r="R59" s="24"/>
@@ -4013,19 +4117,19 @@
       <c r="B60" s="9"/>
       <c r="C60" s="26"/>
       <c r="D60" s="36"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
       <c r="G60" s="25"/>
       <c r="H60" s="25"/>
       <c r="I60" s="25"/>
-      <c r="J60" s="57"/>
-      <c r="K60" s="57"/>
+      <c r="J60" s="68"/>
+      <c r="K60" s="68"/>
       <c r="L60" s="25"/>
       <c r="M60" s="25"/>
       <c r="N60" s="25"/>
-      <c r="O60" s="35"/>
-      <c r="P60" s="35"/>
-      <c r="Q60" s="37"/>
+      <c r="O60" s="38"/>
+      <c r="P60" s="38"/>
+      <c r="Q60" s="39"/>
       <c r="R60" s="28"/>
       <c r="S60" s="12"/>
     </row>
@@ -4034,20 +4138,20 @@
         <v>14</v>
       </c>
       <c r="C61" s="29"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="34"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="37"/>
       <c r="G61" s="25"/>
       <c r="H61" s="25"/>
       <c r="I61" s="25"/>
-      <c r="J61" s="57"/>
-      <c r="K61" s="57"/>
+      <c r="J61" s="68"/>
+      <c r="K61" s="68"/>
       <c r="L61" s="25"/>
       <c r="M61" s="25"/>
       <c r="N61" s="25"/>
-      <c r="O61" s="35"/>
-      <c r="P61" s="35"/>
-      <c r="Q61" s="25"/>
+      <c r="O61" s="38"/>
+      <c r="P61" s="38"/>
+      <c r="Q61" s="40"/>
       <c r="R61" s="32"/>
       <c r="S61" s="12" t="n">
         <v>14</v>
@@ -4056,20 +4160,20 @@
     <row r="62" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="9"/>
       <c r="C62" s="33"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="34"/>
-      <c r="F62" s="36"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="46"/>
       <c r="G62" s="25"/>
       <c r="H62" s="25"/>
       <c r="I62" s="25"/>
-      <c r="J62" s="57"/>
-      <c r="K62" s="57"/>
+      <c r="J62" s="68"/>
+      <c r="K62" s="68"/>
       <c r="L62" s="25"/>
       <c r="M62" s="25"/>
       <c r="N62" s="25"/>
-      <c r="O62" s="37"/>
-      <c r="P62" s="35"/>
-      <c r="Q62" s="25"/>
+      <c r="O62" s="48"/>
+      <c r="P62" s="38"/>
+      <c r="Q62" s="40"/>
       <c r="R62" s="33"/>
       <c r="S62" s="12"/>
     </row>
@@ -4078,20 +4182,20 @@
         <v>7</v>
       </c>
       <c r="C63" s="24"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="34"/>
+      <c r="D63" s="40"/>
+      <c r="E63" s="37"/>
       <c r="F63" s="25"/>
       <c r="G63" s="25"/>
       <c r="H63" s="25"/>
       <c r="I63" s="25"/>
-      <c r="J63" s="57"/>
-      <c r="K63" s="57"/>
+      <c r="J63" s="68"/>
+      <c r="K63" s="68"/>
       <c r="L63" s="25"/>
       <c r="M63" s="25"/>
       <c r="N63" s="25"/>
       <c r="O63" s="25"/>
-      <c r="P63" s="35"/>
-      <c r="Q63" s="25"/>
+      <c r="P63" s="38"/>
+      <c r="Q63" s="40"/>
       <c r="R63" s="24"/>
       <c r="S63" s="12" t="n">
         <v>7</v>
@@ -4100,20 +4204,20 @@
     <row r="64" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B64" s="9"/>
       <c r="C64" s="26"/>
-      <c r="D64" s="27"/>
-      <c r="E64" s="34"/>
+      <c r="D64" s="43"/>
+      <c r="E64" s="37"/>
       <c r="F64" s="25"/>
       <c r="G64" s="25"/>
       <c r="H64" s="25"/>
       <c r="I64" s="25"/>
-      <c r="J64" s="57"/>
-      <c r="K64" s="57"/>
+      <c r="J64" s="68"/>
+      <c r="K64" s="68"/>
       <c r="L64" s="25"/>
       <c r="M64" s="25"/>
       <c r="N64" s="25"/>
       <c r="O64" s="25"/>
-      <c r="P64" s="35"/>
-      <c r="Q64" s="27"/>
+      <c r="P64" s="38"/>
+      <c r="Q64" s="43"/>
       <c r="R64" s="28"/>
       <c r="S64" s="12"/>
     </row>
@@ -4122,20 +4226,20 @@
         <v>10</v>
       </c>
       <c r="C65" s="29"/>
-      <c r="D65" s="30"/>
-      <c r="E65" s="34"/>
+      <c r="D65" s="44"/>
+      <c r="E65" s="37"/>
       <c r="F65" s="25"/>
       <c r="G65" s="25"/>
       <c r="H65" s="25"/>
       <c r="I65" s="25"/>
-      <c r="J65" s="57"/>
-      <c r="K65" s="57"/>
+      <c r="J65" s="68"/>
+      <c r="K65" s="68"/>
       <c r="L65" s="25"/>
       <c r="M65" s="25"/>
       <c r="N65" s="25"/>
       <c r="O65" s="25"/>
-      <c r="P65" s="35"/>
-      <c r="Q65" s="31"/>
+      <c r="P65" s="38"/>
+      <c r="Q65" s="45"/>
       <c r="R65" s="32"/>
       <c r="S65" s="12" t="n">
         <v>10</v>
@@ -4145,18 +4249,18 @@
       <c r="B66" s="9"/>
       <c r="C66" s="33"/>
       <c r="D66" s="34"/>
-      <c r="E66" s="36"/>
+      <c r="E66" s="46"/>
       <c r="F66" s="25"/>
       <c r="G66" s="25"/>
       <c r="H66" s="25"/>
       <c r="I66" s="25"/>
-      <c r="J66" s="57"/>
-      <c r="K66" s="57"/>
+      <c r="J66" s="68"/>
+      <c r="K66" s="68"/>
       <c r="L66" s="25"/>
       <c r="M66" s="25"/>
       <c r="N66" s="25"/>
       <c r="O66" s="25"/>
-      <c r="P66" s="37"/>
+      <c r="P66" s="48"/>
       <c r="Q66" s="35"/>
       <c r="R66" s="33"/>
       <c r="S66" s="12"/>
@@ -4172,8 +4276,8 @@
       <c r="G67" s="25"/>
       <c r="H67" s="25"/>
       <c r="I67" s="25"/>
-      <c r="J67" s="57"/>
-      <c r="K67" s="57"/>
+      <c r="J67" s="68"/>
+      <c r="K67" s="68"/>
       <c r="L67" s="25"/>
       <c r="M67" s="25"/>
       <c r="N67" s="25"/>
@@ -4188,7 +4292,7 @@
     <row r="68" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B68" s="9"/>
       <c r="C68" s="26"/>
-      <c r="D68" s="36"/>
+      <c r="D68" s="46"/>
       <c r="E68" s="25"/>
       <c r="F68" s="25"/>
       <c r="G68" s="25"/>
@@ -4201,12 +4305,12 @@
       <c r="N68" s="25"/>
       <c r="O68" s="25"/>
       <c r="P68" s="25"/>
-      <c r="Q68" s="37"/>
+      <c r="Q68" s="48"/>
       <c r="R68" s="28"/>
       <c r="S68" s="12"/>
     </row>
     <row r="69" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B69" s="9" t="n">
+      <c r="B69" s="69" t="n">
         <v>15</v>
       </c>
       <c r="C69" s="29"/>
@@ -4225,101 +4329,125 @@
       <c r="P69" s="25"/>
       <c r="Q69" s="25"/>
       <c r="R69" s="32"/>
-      <c r="S69" s="12" t="n">
+      <c r="S69" s="70" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="10"/>
-      <c r="C70" s="58"/>
-      <c r="D70" s="58"/>
-      <c r="E70" s="58"/>
-      <c r="F70" s="58"/>
-      <c r="G70" s="58"/>
-      <c r="H70" s="58"/>
-      <c r="I70" s="58"/>
-      <c r="J70" s="58"/>
-      <c r="K70" s="58"/>
-      <c r="L70" s="58"/>
-      <c r="M70" s="58"/>
-      <c r="N70" s="58"/>
-      <c r="O70" s="58"/>
-      <c r="P70" s="58"/>
-      <c r="Q70" s="58"/>
-      <c r="R70" s="58"/>
-      <c r="S70" s="10"/>
+      <c r="B70" s="69"/>
+      <c r="C70" s="71"/>
+      <c r="D70" s="71"/>
+      <c r="E70" s="71"/>
+      <c r="F70" s="71"/>
+      <c r="G70" s="71"/>
+      <c r="H70" s="71"/>
+      <c r="I70" s="71"/>
+      <c r="J70" s="71"/>
+      <c r="K70" s="71"/>
+      <c r="L70" s="71"/>
+      <c r="M70" s="71"/>
+      <c r="N70" s="71"/>
+      <c r="O70" s="71"/>
+      <c r="P70" s="71"/>
+      <c r="Q70" s="71"/>
+      <c r="R70" s="71"/>
+      <c r="S70" s="70"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="59"/>
-      <c r="C71" s="58" t="n">
+      <c r="B71" s="72"/>
+      <c r="C71" s="71" t="n">
         <v>11</v>
       </c>
       <c r="D71" s="24"/>
-      <c r="E71" s="60" t="n">
+      <c r="E71" s="73" t="n">
         <v>16</v>
       </c>
-      <c r="F71" s="61"/>
-      <c r="G71" s="58"/>
-      <c r="H71" s="58"/>
-      <c r="I71" s="58"/>
-      <c r="J71" s="62"/>
-      <c r="K71" s="58"/>
-      <c r="L71" s="58"/>
-      <c r="M71" s="58"/>
-      <c r="N71" s="58"/>
-      <c r="O71" s="61"/>
-      <c r="P71" s="63" t="n">
+      <c r="F71" s="74"/>
+      <c r="G71" s="71"/>
+      <c r="H71" s="71"/>
+      <c r="I71" s="71"/>
+      <c r="J71" s="75"/>
+      <c r="K71" s="71"/>
+      <c r="L71" s="71"/>
+      <c r="M71" s="71"/>
+      <c r="N71" s="71"/>
+      <c r="O71" s="74"/>
+      <c r="P71" s="76" t="n">
         <v>16</v>
       </c>
-      <c r="Q71" s="61"/>
-      <c r="R71" s="63" t="n">
+      <c r="Q71" s="74"/>
+      <c r="R71" s="76" t="n">
         <v>11</v>
       </c>
-      <c r="S71" s="59"/>
+      <c r="S71" s="77"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C72" s="64"/>
+      <c r="B72" s="78"/>
+      <c r="C72" s="79"/>
       <c r="D72" s="26"/>
-      <c r="E72" s="65"/>
-      <c r="F72" s="64"/>
-      <c r="G72" s="66"/>
-      <c r="H72" s="61"/>
-      <c r="I72" s="64"/>
-      <c r="J72" s="64"/>
-      <c r="K72" s="64"/>
-      <c r="L72" s="64"/>
-      <c r="M72" s="61"/>
-      <c r="N72" s="61"/>
-      <c r="O72" s="67"/>
-      <c r="P72" s="61"/>
-      <c r="Q72" s="67"/>
-      <c r="R72" s="58"/>
+      <c r="E72" s="80"/>
+      <c r="F72" s="79"/>
+      <c r="G72" s="81"/>
+      <c r="H72" s="74"/>
+      <c r="I72" s="79"/>
+      <c r="J72" s="79"/>
+      <c r="K72" s="79"/>
+      <c r="L72" s="79"/>
+      <c r="M72" s="74"/>
+      <c r="N72" s="74"/>
+      <c r="O72" s="82"/>
+      <c r="P72" s="74"/>
+      <c r="Q72" s="82"/>
+      <c r="R72" s="71"/>
+      <c r="S72" s="83"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C73" s="64" t="n">
+      <c r="B73" s="78"/>
+      <c r="C73" s="79" t="n">
         <v>11</v>
       </c>
       <c r="D73" s="29"/>
-      <c r="E73" s="60" t="n">
+      <c r="E73" s="73" t="n">
         <v>16</v>
       </c>
-      <c r="F73" s="61"/>
-      <c r="G73" s="67"/>
-      <c r="H73" s="64"/>
-      <c r="I73" s="64"/>
-      <c r="J73" s="64"/>
-      <c r="K73" s="64"/>
-      <c r="L73" s="64"/>
-      <c r="M73" s="58"/>
-      <c r="N73" s="58"/>
-      <c r="O73" s="66"/>
-      <c r="P73" s="63" t="n">
+      <c r="F73" s="74"/>
+      <c r="G73" s="82"/>
+      <c r="H73" s="79"/>
+      <c r="I73" s="79"/>
+      <c r="J73" s="79"/>
+      <c r="K73" s="79"/>
+      <c r="L73" s="79"/>
+      <c r="M73" s="71"/>
+      <c r="N73" s="71"/>
+      <c r="O73" s="81"/>
+      <c r="P73" s="76" t="n">
         <v>16</v>
       </c>
-      <c r="Q73" s="66"/>
-      <c r="R73" s="63" t="n">
+      <c r="Q73" s="81"/>
+      <c r="R73" s="76" t="n">
         <v>11</v>
       </c>
+      <c r="S73" s="83"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="84"/>
+      <c r="C74" s="85"/>
+      <c r="D74" s="85"/>
+      <c r="E74" s="85"/>
+      <c r="F74" s="85"/>
+      <c r="G74" s="85"/>
+      <c r="H74" s="85"/>
+      <c r="I74" s="85"/>
+      <c r="J74" s="85"/>
+      <c r="K74" s="85"/>
+      <c r="L74" s="85"/>
+      <c r="M74" s="85"/>
+      <c r="N74" s="85"/>
+      <c r="O74" s="85"/>
+      <c r="P74" s="85"/>
+      <c r="Q74" s="85"/>
+      <c r="R74" s="85"/>
+      <c r="S74" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="40">
@@ -4366,7 +4494,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>